<commit_message>
save celebration to record_file and show to  app windows
</commit_message>
<xml_diff>
--- a/related_files/celebration_text.xlsx
+++ b/related_files/celebration_text.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\py_project\birthday\related_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2656D3DD-C285-4084-B2C8-DB1EFDD2589D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0B31B0-E665-4E83-BEB6-DBD3D31606A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26388" yWindow="3444" windowWidth="17280" windowHeight="9036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,17 +25,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>生日祝福</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>生日快乐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>生日快乐哈哈哈</t>
+    <t>生日快乐哈哈哈1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日快乐2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日快乐哈哈哈3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日快乐4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日快乐哈哈哈5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日快乐6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日快乐哈哈哈7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日快乐8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日快乐9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日快乐哈哈哈10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生日快乐0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -361,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A36"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -379,177 +415,57 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>